<commit_message>
test login - done!
</commit_message>
<xml_diff>
--- a/LazadaSeleniumWebdriver/lazadaTestData/TestDataLazada.xlsx
+++ b/LazadaSeleniumWebdriver/lazadaTestData/TestDataLazada.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13560" windowHeight="6060" firstSheet="1" activeTab="1"/>
+    <workbookView activeTab="2" firstSheet="2" windowHeight="6060" windowWidth="13560" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="1. Trang chủ" sheetId="4" r:id="rId1"/>
-    <sheet name="2.1. ĐN_Kiểm tra links" sheetId="1" r:id="rId2"/>
-    <sheet name="2.2. ĐN_Form đăng nhập" sheetId="5" r:id="rId3"/>
-    <sheet name="2.3. ĐN_Tài khoản liên kết" sheetId="6" r:id="rId4"/>
-    <sheet name="3. Đăng ký" sheetId="2" r:id="rId5"/>
-    <sheet name="4. Quên mật khẩu" sheetId="3" r:id="rId6"/>
+    <sheet name="1. Trang chủ" r:id="rId1" sheetId="4"/>
+    <sheet name="2.1. ĐN_Kiểm tra links" r:id="rId2" sheetId="1"/>
+    <sheet name="2.2. ĐN_Form đăng nhập" r:id="rId3" sheetId="5"/>
+    <sheet name="2.3. ĐN_Tài khoản liên kết" r:id="rId4" sheetId="6"/>
+    <sheet name="3. Đăng ký" r:id="rId5" sheetId="2"/>
+    <sheet name="4. Quên mật khẩu" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>Email</t>
   </si>
@@ -75,82 +75,86 @@
     <t>Quên mật khẩu?</t>
   </si>
   <si>
+    <t>Lazada - Create new customer account</t>
+  </si>
+  <si>
+    <t>ĐN_08</t>
+  </si>
+  <si>
+    <t>ĐN_09</t>
+  </si>
+  <si>
+    <t>ĐN_10</t>
+  </si>
+  <si>
+    <t>ĐN_11</t>
+  </si>
+  <si>
+    <t>ĐN_12</t>
+  </si>
+  <si>
+    <t>ĐN_13</t>
+  </si>
+  <si>
+    <t>test3.duongntt@hotmail.com</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>duongntt_d8cnpm@epu.edu.vn</t>
+  </si>
+  <si>
+    <t>ĐN_14</t>
+  </si>
+  <si>
+    <t>ĐN_15</t>
+  </si>
+  <si>
+    <t>ĐN_18</t>
+  </si>
+  <si>
+    <t>ĐN_19</t>
+  </si>
+  <si>
+    <t>test2.duongntt@gmail.com</t>
+  </si>
+  <si>
+    <t>Social media</t>
+  </si>
+  <si>
+    <t>Google+</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Lazada - My account</t>
+  </si>
+  <si>
+    <t>Lazada - Login</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Đăng kí ngay!</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>Lazada - Forgot password?</t>
-  </si>
-  <si>
-    <t>Lazada - Create new customer account</t>
-  </si>
-  <si>
-    <t>ĐN_08</t>
-  </si>
-  <si>
-    <t>ĐN_09</t>
-  </si>
-  <si>
-    <t>ĐN_10</t>
-  </si>
-  <si>
-    <t>ĐN_11</t>
-  </si>
-  <si>
-    <t>ĐN_12</t>
-  </si>
-  <si>
-    <t>ĐN_13</t>
-  </si>
-  <si>
-    <t>test3.duongntt@hotmail.com</t>
-  </si>
-  <si>
-    <t>abc123</t>
-  </si>
-  <si>
-    <t>duongntt_d8cnpm@epu.edu.vn</t>
-  </si>
-  <si>
-    <t>ĐN_14</t>
-  </si>
-  <si>
-    <t>ĐN_15</t>
-  </si>
-  <si>
-    <t>ĐN_18</t>
-  </si>
-  <si>
-    <t>ĐN_19</t>
-  </si>
-  <si>
-    <t>test2.duongntt@gmail.com</t>
-  </si>
-  <si>
-    <t>Social media</t>
-  </si>
-  <si>
-    <t>Google+</t>
-  </si>
-  <si>
-    <t>Facebook</t>
-  </si>
-  <si>
-    <t>Lazada - My account</t>
-  </si>
-  <si>
-    <t>Lazada - Login</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Đăng kí ngay!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -240,52 +244,52 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -302,10 +306,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -340,7 +344,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,7 +379,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -463,7 +467,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -472,13 +476,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -488,7 +492,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -497,7 +501,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -506,7 +510,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -516,12 +520,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -552,7 +556,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -571,7 +575,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -583,7 +587,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -592,35 +596,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="40" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="40.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
   </cols>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="40" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="40.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -634,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -645,7 +649,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>40</v>
@@ -656,38 +660,38 @@
         <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="40" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="40.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -710,12 +714,12 @@
         <v>14</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -730,15 +734,15 @@
         <v>4</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -749,15 +753,15 @@
         <v>4</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
@@ -768,15 +772,15 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -789,15 +793,15 @@
         <v>6</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
@@ -810,39 +814,39 @@
         <v>6</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -852,7 +856,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>40</v>
@@ -860,7 +864,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -871,42 +875,42 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B6" r:id="rId6"/>
+    <hyperlink r:id="rId1" ref="B3"/>
+    <hyperlink r:id="rId2" ref="B5"/>
+    <hyperlink r:id="rId3" ref="B7"/>
+    <hyperlink r:id="rId4" ref="B8"/>
+    <hyperlink r:id="rId5" ref="B9"/>
+    <hyperlink r:id="rId6" ref="B6"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId7" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.765625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -914,7 +918,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -926,75 +930,79 @@
         <v>14</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="C3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId3" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>